<commit_message>
fix: Exc. mortality by Andras
</commit_message>
<xml_diff>
--- a/02_Data/02_Pandemic variables/03_Exc. Mortality/EM_Data_availability.xlsx
+++ b/02_Data/02_Pandemic variables/03_Exc. Mortality/EM_Data_availability.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Dropbox (HÉTFA)\ESPON_COVID19\2021\04_SZAKMAI ANYAGOK\01_Geography_of_Covid-19\Databases\Common data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6547F54E-2262-4DB4-9546-626C68F39B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3FD6DB-E488-4483-AAFC-4FC7528645F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data status" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miH3cUAJo23w6D4wSIpuK9G5stdbQ=="/>
     </ext>
@@ -25,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="86">
   <si>
     <t xml:space="preserve">Y: Exc. Mortality </t>
   </si>
@@ -153,24 +160,9 @@
     <t>01.01.2020. to 31.10.2021.</t>
   </si>
   <si>
-    <t>01.01.2020. to 24.10.2021.</t>
-  </si>
-  <si>
-    <t>01.01.2020. to 03.10.2021.</t>
-  </si>
-  <si>
     <t>NUTS1</t>
   </si>
   <si>
-    <t>01.01.2020. to 05.09.2021.</t>
-  </si>
-  <si>
-    <t>01.01.2020. to 26.09.2021.</t>
-  </si>
-  <si>
-    <t>01.01.2020. to 17.10.2021.</t>
-  </si>
-  <si>
     <t>England, Wales (UK)</t>
   </si>
   <si>
@@ -183,9 +175,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>weekly NUTS3 level data are available until the end of 2020</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -300,7 +289,7 @@
     <t>Data of 5 regions is estimated based on data of local authorities</t>
   </si>
   <si>
-    <t>the value for the reference period (2015-2019) is based on an estimation (from monthly data)</t>
+    <t>weekly NUTS3 level data are available until the end of 2020; NUTS1 = NUTS0</t>
   </si>
 </sst>
 </file>
@@ -318,17 +307,23 @@
       <sz val="11"/>
       <color rgb="FF585858"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Georgia"/>
+      <family val="1"/>
+      <charset val="238"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Georgia"/>
+      <family val="1"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="11"/>
@@ -408,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -422,6 +417,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -639,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -694,7 +690,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
@@ -706,7 +702,7 @@
         <v>5</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
@@ -714,7 +710,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>7</v>
@@ -726,7 +722,7 @@
         <v>8</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
@@ -734,7 +730,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>7</v>
@@ -746,7 +742,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
@@ -754,7 +750,7 @@
         <v>34</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>7</v>
@@ -772,7 +768,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>7</v>
@@ -784,7 +780,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
@@ -792,19 +788,19 @@
         <v>35</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>43</v>
+      <c r="D8" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
@@ -812,19 +808,19 @@
         <v>11</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>42</v>
+      <c r="D9" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
@@ -832,10 +828,10 @@
         <v>12</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>41</v>
@@ -844,7 +840,7 @@
         <v>8</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
@@ -852,7 +848,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>7</v>
@@ -864,7 +860,7 @@
         <v>8</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
@@ -872,10 +868,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>41</v>
@@ -884,7 +880,7 @@
         <v>8</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
@@ -892,19 +888,19 @@
         <v>15</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>43</v>
+      <c r="D13" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
@@ -912,19 +908,19 @@
         <v>16</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>42</v>
+      <c r="D14" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
@@ -932,7 +928,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>7</v>
@@ -944,7 +940,7 @@
         <v>8</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
@@ -952,7 +948,7 @@
         <v>18</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>7</v>
@@ -964,7 +960,7 @@
         <v>8</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
@@ -972,10 +968,10 @@
         <v>19</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>41</v>
@@ -984,7 +980,7 @@
         <v>8</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
@@ -992,7 +988,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>7</v>
@@ -1004,27 +1000,27 @@
         <v>8</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>45</v>
+        <v>58</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="10" t="s">
-        <v>91</v>
+      <c r="F19" s="9" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
@@ -1032,7 +1028,7 @@
         <v>39</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>7</v>
@@ -1044,7 +1040,7 @@
         <v>8</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1052,19 +1048,19 @@
         <v>22</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>43</v>
+      <c r="D21" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1072,7 +1068,7 @@
         <v>40</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>7</v>
@@ -1084,7 +1080,7 @@
         <v>8</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1092,7 +1088,7 @@
         <v>36</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>7</v>
@@ -1104,7 +1100,7 @@
         <v>8</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1112,7 +1108,7 @@
         <v>37</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>7</v>
@@ -1124,7 +1120,7 @@
         <v>8</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1132,7 +1128,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>7</v>
@@ -1144,7 +1140,7 @@
         <v>8</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1152,10 +1148,10 @@
         <v>38</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>41</v>
@@ -1164,7 +1160,7 @@
         <v>8</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
@@ -1172,7 +1168,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>7</v>
@@ -1184,7 +1180,7 @@
         <v>8</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
@@ -1192,7 +1188,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>7</v>
@@ -1204,7 +1200,7 @@
         <v>8</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1212,7 +1208,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>27</v>
@@ -1224,7 +1220,7 @@
         <v>8</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1232,7 +1228,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>7</v>
@@ -1244,7 +1240,7 @@
         <v>8</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1252,19 +1248,19 @@
         <v>29</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1272,7 +1268,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>7</v>
@@ -1284,7 +1280,7 @@
         <v>8</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1292,19 +1288,19 @@
         <v>31</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="E33" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1312,7 +1308,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>7</v>
@@ -1324,15 +1320,15 @@
         <v>8</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>7</v>
@@ -1344,7 +1340,7 @@
         <v>8</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
@@ -1352,27 +1348,27 @@
         <v>32</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>7</v>
@@ -1384,7 +1380,7 @@
         <v>8</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>